<commit_message>
reorganize ChapmanHall/ a bit
</commit_message>
<xml_diff>
--- a/ChapmanHall/FixArt_candidates.xlsx
+++ b/ChapmanHall/FixArt_candidates.xlsx
@@ -1009,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -1017,7 +1017,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fixed figs in Ch07; avoid deprecated effects:: warning in Ch11
</commit_message>
<xml_diff>
--- a/ChapmanHall/FixArt_candidates.xlsx
+++ b/ChapmanHall/FixArt_candidates.xlsx
@@ -366,9 +366,6 @@
     <t>May look better if the y axis label is put further from scale labels</t>
   </si>
   <si>
-    <t>FIXME: should use theme_bw()</t>
-  </si>
-  <si>
     <t>7.7</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>nmes2-eff1</t>
+  </si>
+  <si>
+    <t>fixed + theme_bw()</t>
   </si>
 </sst>
 </file>
@@ -624,17 +624,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -652,14 +652,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -672,9 +671,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -686,12 +686,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1061,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1616,30 +1617,30 @@
       <c r="C39" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>116</v>
+      <c r="D39" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" t="s">
         <v>117</v>
-      </c>
-      <c r="B40" t="s">
-        <v>118</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>116</v>
+      <c r="D40" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
         <v>119</v>
-      </c>
-      <c r="B41" t="s">
-        <v>120</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>115</v>
@@ -1650,13 +1651,13 @@
     </row>
     <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
         <v>121</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="D42" t="s">
         <v>67</v>
@@ -1664,41 +1665,41 @@
     </row>
     <row r="43" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" t="s">
         <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>125</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>116</v>
+      <c r="D43" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" t="s">
         <v>126</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>116</v>
+      <c r="D44" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" t="s">
         <v>128</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -1706,13 +1707,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" t="s">
         <v>131</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -1720,139 +1721,139 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" t="s">
         <v>134</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" t="s">
         <v>137</v>
       </c>
-      <c r="B48" t="s">
-        <v>138</v>
-      </c>
       <c r="C48" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
         <v>139</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" t="s">
-        <v>143</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" t="s">
-        <v>145</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" t="s">
-        <v>147</v>
-      </c>
       <c r="C52" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D52" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
         <v>148</v>
-      </c>
-      <c r="B53" t="s">
-        <v>149</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" t="s">
         <v>150</v>
-      </c>
-      <c r="B54" t="s">
-        <v>151</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" t="s">
         <v>152</v>
       </c>
-      <c r="B55" t="s">
-        <v>153</v>
-      </c>
       <c r="C55" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" t="s">
         <v>154</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>33</v>
@@ -1860,13 +1861,13 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" t="s">
         <v>157</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>33</v>
@@ -1874,27 +1875,27 @@
     </row>
     <row r="58" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" t="s">
         <v>163</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>33</v>
@@ -1902,13 +1903,13 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60" t="s">
         <v>166</v>
       </c>
-      <c r="B60" t="s">
-        <v>167</v>
-      </c>
       <c r="C60" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>33</v>
@@ -1916,155 +1917,155 @@
     </row>
     <row r="61" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" t="s">
         <v>168</v>
-      </c>
-      <c r="B61" t="s">
-        <v>169</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
         <v>170</v>
-      </c>
-      <c r="B62" t="s">
-        <v>171</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" t="s">
         <v>172</v>
       </c>
-      <c r="B63" t="s">
-        <v>173</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D63" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" t="s">
         <v>174</v>
       </c>
-      <c r="B64" t="s">
-        <v>175</v>
-      </c>
       <c r="C64" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D64" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" t="s">
         <v>176</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="D65" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" t="s">
         <v>180</v>
       </c>
-      <c r="B66" t="s">
-        <v>181</v>
-      </c>
       <c r="C66" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D66" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B67" t="s">
         <v>182</v>
       </c>
-      <c r="B67" t="s">
-        <v>183</v>
-      </c>
       <c r="C67" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" t="s">
         <v>184</v>
       </c>
-      <c r="B68" t="s">
-        <v>185</v>
-      </c>
       <c r="C68" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D68" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B69" t="s">
         <v>186</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" t="s">
         <v>189</v>
-      </c>
-      <c r="B70" t="s">
-        <v>190</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B71" t="s">
         <v>191</v>
       </c>
-      <c r="B71" t="s">
-        <v>192</v>
-      </c>
       <c r="C71" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D71" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>